<commit_message>
Add documentation and update to threads part to run one at a time
</commit_message>
<xml_diff>
--- a/Resource/BOLETIN.xlsx
+++ b/Resource/BOLETIN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Telegram Desktop\Proyecto-carlobranch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Proyecto\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCD3513-6953-4680-B63B-4627F75ED8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A99FFC-1304-4550-9A2F-A9E5D6758244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,38 +382,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -428,30 +405,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -468,22 +494,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>297366</xdr:colOff>
+      <xdr:colOff>254781</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>42559</xdr:rowOff>
+      <xdr:rowOff>28373</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>376363</xdr:colOff>
+      <xdr:colOff>346158</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>157976</xdr:rowOff>
+      <xdr:rowOff>170916</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A8E7D7-3BC6-EE6D-8051-32E5836D58B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BD0E5B5-0BEC-8020-B295-4F5BAB259CC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -505,8 +531,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="297366" y="42559"/>
-          <a:ext cx="785241" cy="659039"/>
+          <a:off x="254781" y="28373"/>
+          <a:ext cx="796632" cy="689724"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -837,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="235" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="235" workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,404 +880,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
+      <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="23" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="7"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="5" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="39" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="6"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="6"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="38"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="3"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="25" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="25" t="s">
+      <c r="D27" s="17"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A5:H5"/>
@@ -1276,6 +1303,7 @@
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.86" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Community Service Project update
</commit_message>
<xml_diff>
--- a/Resource/BOLETIN.xlsx
+++ b/Resource/BOLETIN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Proyecto\Resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\NotasExpress\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A99FFC-1304-4550-9A2F-A9E5D6758244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A273548-A2BF-49E3-BF05-4D0F9DF75F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -391,6 +391,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -405,67 +428,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,293 +869,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="22"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7" t="s">
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="28"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="39" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="38"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="42"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="38"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="38"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="38"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="38"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="38"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="38"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="38"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1183,16 +1160,18 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="A22" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1237,30 +1216,30 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -1278,7 +1257,7 @@
       <c r="K28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A5:H5"/>
@@ -1287,10 +1266,12 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A22:J22"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
     <mergeCell ref="C1:K3"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A13:G13"/>

</xml_diff>

<commit_message>
Community Service Project update 1.1
</commit_message>
<xml_diff>
--- a/Resource/BOLETIN.xlsx
+++ b/Resource/BOLETIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\NotasExpress\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A273548-A2BF-49E3-BF05-4D0F9DF75F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC84E97E-204C-4C7C-BF75-3866E2909CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,17 +403,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -422,6 +415,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -441,18 +453,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:J22"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,9 +869,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="9"/>
@@ -881,111 +881,111 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="23" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="5" t="s">
         <v>2</v>
       </c>
@@ -1000,153 +1000,141 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="6"/>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="6"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="6"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="6"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="6"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="6"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="6"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="6"/>
       <c r="K16" s="4"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
+    <row r="17" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="6"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="6"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1159,22 +1147,22 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1187,7 +1175,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1200,7 +1188,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1213,29 +1201,29 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="15"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="28" t="s">
+      <c r="G27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="9"/>
@@ -1243,7 +1231,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1257,7 +1245,20 @@
       <c r="K28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="26">
+    <mergeCell ref="C1:K3"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A7:K7"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A5:H5"/>
@@ -1271,20 +1272,6 @@
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="C1:K3"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.86" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>

</xml_diff>